<commit_message>
Update "Pesquisa de referências"
</commit_message>
<xml_diff>
--- a/DocsRequisitos/Pesquisa de referências.xlsx
+++ b/DocsRequisitos/Pesquisa de referências.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6748A209-2476-4FAA-B9C5-4F5E7ECF281B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BFD15D-CF40-4776-8D10-F606C9F84AC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{53AF8882-0C28-4C83-B0B2-CDF784B39E5B}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Controle do rotativo</t>
-  </si>
-  <si>
-    <t>&gt; Controla a entrada e saida dos carros</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>&gt;Auto peenche dados de clientes frequentes</t>
   </si>
@@ -43,6 +37,57 @@
   </si>
   <si>
     <t>JumpPark:</t>
+  </si>
+  <si>
+    <t>&gt;Realiza todas as transações nescessárias</t>
+  </si>
+  <si>
+    <t>&gt;Controla a entrada e saida dos carros</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&gt;todas são transacionadas com saldo positivo ou negativo</t>
+  </si>
+  <si>
+    <t>&gt;Recibo de pagamento</t>
+  </si>
+  <si>
+    <t>&gt;Aviso de entrada e saida</t>
+  </si>
+  <si>
+    <t>&gt;Inicio e fim dos serviços</t>
+  </si>
+  <si>
+    <t>&gt;Mapeamento do veículo na entrada utilizando fotos</t>
+  </si>
+  <si>
+    <t>&gt;Idependencia de internet durante o uso do programa</t>
+  </si>
+  <si>
+    <t>&gt;Inclusão de serviços automotivos</t>
+  </si>
+  <si>
+    <t>&gt;Checklist de avaria dos veículos</t>
+  </si>
+  <si>
+    <t>&gt;Comunicação por email</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>&gt;Controle de convênios ou pós-pago</t>
+  </si>
+  <si>
+    <t>&gt;Geração de relatórios detalhados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;Envio de recibos das faturas por e-mail </t>
+  </si>
+  <si>
+    <t>https://jumppark.com.br/</t>
   </si>
 </sst>
 </file>
@@ -56,11 +101,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <b/>
@@ -76,6 +116,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,20 +143,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,49 +469,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2716AADC-C428-4D22-B545-4445C5DF869F}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{0D6F8800-50D5-4847-A8B3-312226DCFF9A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>